<commit_message>
changes for showing stats of latest dates
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -58,7 +58,7 @@
     <t>linkedin</t>
   </si>
   <si>
-    <t>09/20/2024</t>
+    <t>09/21/2024</t>
   </si>
   <si>
     <t>NA</t>
@@ -94,10 +94,10 @@
     <t>zeniva</t>
   </si>
   <si>
-    <t>09/21/2024</t>
+    <t>09/22/2024</t>
   </si>
   <si>
-    <t>09/22/2024</t>
+    <t>09/23/2024</t>
   </si>
   <si>
     <t>Product</t>
@@ -173,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -198,17 +198,23 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -500,10 +506,10 @@
         <v>15</v>
       </c>
       <c r="G2" s="3">
-        <v>10032.0</v>
+        <v>10034.0</v>
       </c>
       <c r="H2" s="4">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="I2" s="4">
         <v>4.0</v>
@@ -764,7 +770,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="3">
-        <v>265.0</v>
+        <v>300.0</v>
       </c>
       <c r="E9" s="3">
         <v>1000.0</v>
@@ -782,7 +788,7 @@
         <v>15</v>
       </c>
       <c r="J9" s="3">
-        <v>28966.0</v>
+        <v>31166.0</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>15</v>
@@ -803,7 +809,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="3">
-        <v>54.0</v>
+        <v>59.0</v>
       </c>
       <c r="E10" s="3">
         <v>3680.0</v>
@@ -827,7 +833,7 @@
         <v>15</v>
       </c>
       <c r="L10" s="3">
-        <v>1860.0</v>
+        <v>2200.0</v>
       </c>
       <c r="M10" s="2"/>
     </row>
@@ -842,7 +848,7 @@
         <v>14</v>
       </c>
       <c r="D11" s="3">
-        <v>61.0</v>
+        <v>62.0</v>
       </c>
       <c r="E11" s="3">
         <v>2784.0</v>
@@ -863,10 +869,10 @@
         <v>15</v>
       </c>
       <c r="K11" s="3">
-        <v>9.0</v>
+        <v>3.0</v>
       </c>
       <c r="L11" s="3">
-        <v>2208.0</v>
+        <v>2269.0</v>
       </c>
       <c r="M11" s="2"/>
     </row>
@@ -920,13 +926,13 @@
         <v>14</v>
       </c>
       <c r="D13" s="3">
-        <v>79.0</v>
+        <v>84.0</v>
       </c>
       <c r="E13" s="3">
         <v>1635.0</v>
       </c>
       <c r="F13" s="3">
-        <v>10700.0</v>
+        <v>13300.0</v>
       </c>
       <c r="G13" s="3">
         <v>581.0</v>
@@ -970,8 +976,8 @@
       <c r="G14" s="3">
         <v>65.0</v>
       </c>
-      <c r="H14" s="3">
-        <v>1.0</v>
+      <c r="H14" s="4">
+        <v>0.0</v>
       </c>
       <c r="I14" s="3">
         <v>0.0</v>
@@ -1013,7 +1019,7 @@
         <v>0.0</v>
       </c>
       <c r="I15" s="4">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>15</v>
@@ -1085,13 +1091,13 @@
         <v>15</v>
       </c>
       <c r="G17" s="3">
-        <v>1559.0</v>
+        <v>1560.0</v>
       </c>
       <c r="H17" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="I17" s="3">
         <v>1.0</v>
-      </c>
-      <c r="I17" s="3">
-        <v>2.0</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>15</v>
@@ -1133,7 +1139,7 @@
         <v>15</v>
       </c>
       <c r="J18" s="3">
-        <v>22236.0</v>
+        <v>26233.0</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>15</v>
@@ -1154,7 +1160,7 @@
         <v>14</v>
       </c>
       <c r="D19" s="3">
-        <v>137.0</v>
+        <v>208.0</v>
       </c>
       <c r="E19" s="3">
         <v>3500.0</v>
@@ -1178,7 +1184,7 @@
         <v>15</v>
       </c>
       <c r="L19" s="3">
-        <v>888.0</v>
+        <v>1300.0</v>
       </c>
       <c r="M19" s="2"/>
     </row>
@@ -1217,7 +1223,7 @@
         <v>0.0</v>
       </c>
       <c r="L20" s="3">
-        <v>2121.0</v>
+        <v>2173.0</v>
       </c>
       <c r="M20" s="2"/>
     </row>
@@ -1271,13 +1277,13 @@
         <v>14</v>
       </c>
       <c r="D22" s="3">
-        <v>9.0</v>
+        <v>11.0</v>
       </c>
       <c r="E22" s="3">
         <v>2000.0</v>
       </c>
       <c r="F22" s="3">
-        <v>20200.0</v>
+        <v>22300.0</v>
       </c>
       <c r="G22" s="3">
         <v>275.0</v>
@@ -1325,7 +1331,7 @@
         <v>0.0</v>
       </c>
       <c r="I23" s="4">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>15</v>
@@ -1363,8 +1369,8 @@
       <c r="H24" s="4">
         <v>0.0</v>
       </c>
-      <c r="I24" s="3">
-        <v>1.0</v>
+      <c r="I24" s="4">
+        <v>0.0</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>15</v>
@@ -1402,8 +1408,8 @@
       <c r="H25" s="4">
         <v>0.0</v>
       </c>
-      <c r="I25" s="3">
-        <v>1.0</v>
+      <c r="I25" s="4">
+        <v>0.0</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>15</v>
@@ -1429,20 +1435,6 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1531,13 +1523,13 @@
         <v>15</v>
       </c>
       <c r="G2" s="6">
-        <v>10034.0</v>
+        <v>10037.0</v>
       </c>
       <c r="H2" s="7">
+        <v>3.0</v>
+      </c>
+      <c r="I2" s="7">
         <v>2.0</v>
-      </c>
-      <c r="I2" s="7">
-        <v>4.0</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>15</v>
@@ -1583,10 +1575,10 @@
         <v>15</v>
       </c>
       <c r="G3" s="6">
-        <v>16899.0</v>
+        <v>17061.0</v>
       </c>
       <c r="H3" s="7">
-        <v>0.0</v>
+        <v>162.0</v>
       </c>
       <c r="I3" s="7">
         <v>0.0</v>
@@ -1886,7 +1878,7 @@
         <v>26</v>
       </c>
       <c r="D9" s="6">
-        <v>300.0</v>
+        <v>339.0</v>
       </c>
       <c r="E9" s="6">
         <v>1000.0</v>
@@ -1904,7 +1896,7 @@
         <v>15</v>
       </c>
       <c r="J9" s="6">
-        <v>31166.0</v>
+        <v>34144.0</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>15</v>
@@ -1938,7 +1930,7 @@
         <v>26</v>
       </c>
       <c r="D10" s="6">
-        <v>59.0</v>
+        <v>69.0</v>
       </c>
       <c r="E10" s="6">
         <v>3680.0</v>
@@ -1962,7 +1954,7 @@
         <v>15</v>
       </c>
       <c r="L10" s="6">
-        <v>2200.0</v>
+        <v>2900.0</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1990,7 +1982,7 @@
         <v>26</v>
       </c>
       <c r="D11" s="6">
-        <v>62.0</v>
+        <v>67.0</v>
       </c>
       <c r="E11" s="6">
         <v>2784.0</v>
@@ -2011,10 +2003,10 @@
         <v>15</v>
       </c>
       <c r="K11" s="6">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="L11" s="6">
-        <v>2269.0</v>
+        <v>2346.0</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -2094,13 +2086,13 @@
         <v>26</v>
       </c>
       <c r="D13" s="6">
-        <v>84.0</v>
+        <v>86.0</v>
       </c>
       <c r="E13" s="6">
         <v>1635.0</v>
       </c>
       <c r="F13" s="6">
-        <v>13300.0</v>
+        <v>16200.0</v>
       </c>
       <c r="G13" s="6">
         <v>581.0</v>
@@ -2316,8 +2308,8 @@
       <c r="H17" s="7">
         <v>0.0</v>
       </c>
-      <c r="I17" s="6">
-        <v>1.0</v>
+      <c r="I17" s="7">
+        <v>0.0</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>15</v>
@@ -2354,7 +2346,7 @@
         <v>26</v>
       </c>
       <c r="D18" s="6">
-        <v>249.0</v>
+        <v>308.0</v>
       </c>
       <c r="E18" s="6">
         <v>1000.0</v>
@@ -2372,7 +2364,7 @@
         <v>15</v>
       </c>
       <c r="J18" s="6">
-        <v>26233.0</v>
+        <v>27459.0</v>
       </c>
       <c r="K18" s="5" t="s">
         <v>15</v>
@@ -2406,7 +2398,7 @@
         <v>26</v>
       </c>
       <c r="D19" s="6">
-        <v>208.0</v>
+        <v>251.0</v>
       </c>
       <c r="E19" s="6">
         <v>3500.0</v>
@@ -2430,7 +2422,7 @@
         <v>15</v>
       </c>
       <c r="L19" s="6">
-        <v>1300.0</v>
+        <v>1540.0</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -2458,7 +2450,7 @@
         <v>26</v>
       </c>
       <c r="D20" s="6">
-        <v>33.0</v>
+        <v>36.0</v>
       </c>
       <c r="E20" s="6">
         <v>8352.0</v>
@@ -2482,7 +2474,7 @@
         <v>0.0</v>
       </c>
       <c r="L20" s="6">
-        <v>2173.0</v>
+        <v>2217.0</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -2562,13 +2554,13 @@
         <v>26</v>
       </c>
       <c r="D22" s="6">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="E22" s="6">
         <v>2000.0</v>
       </c>
       <c r="F22" s="6">
-        <v>22300.0</v>
+        <v>24700.0</v>
       </c>
       <c r="G22" s="6">
         <v>275.0</v>
@@ -2675,7 +2667,7 @@
         <v>15</v>
       </c>
       <c r="G24" s="6">
-        <v>401.0</v>
+        <v>398.0</v>
       </c>
       <c r="H24" s="7">
         <v>0.0</v>
@@ -2798,45 +2790,48 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="2"/>
@@ -2855,40 +2850,40 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="3">
-        <v>10037.0</v>
-      </c>
-      <c r="H2" s="4">
+      <c r="D2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="6">
+        <v>10045.0</v>
+      </c>
+      <c r="H2" s="7">
+        <v>8.0</v>
+      </c>
+      <c r="I2" s="7">
         <v>3.0</v>
       </c>
-      <c r="I2" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="J2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M2" s="2"/>
@@ -2907,40 +2902,40 @@
       <c r="Z2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="3">
-        <v>17061.0</v>
-      </c>
-      <c r="H3" s="4">
+      <c r="D3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="6">
+        <v>17042.0</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="I3" s="7">
         <v>162.0</v>
       </c>
-      <c r="I3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="J3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="2"/>
@@ -2959,40 +2954,40 @@
       <c r="Z3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="3">
+      <c r="D4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="6">
         <v>866.0</v>
       </c>
-      <c r="H4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="1" t="s">
+      <c r="H4" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M4" s="2"/>
@@ -3011,40 +3006,40 @@
       <c r="Z4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="1" t="s">
+      <c r="D5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M5" s="2"/>
@@ -3063,40 +3058,40 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="D6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="6">
         <v>2934.0</v>
       </c>
-      <c r="H6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" s="1" t="s">
+      <c r="H6" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M6" s="2"/>
@@ -3115,40 +3110,40 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" s="1" t="s">
+      <c r="D7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="2"/>
@@ -3167,40 +3162,40 @@
       <c r="Z7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="3">
+      <c r="D8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="6">
         <v>311.0</v>
       </c>
-      <c r="H8" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I8" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8" s="1" t="s">
+      <c r="H8" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M8" s="2"/>
@@ -3219,40 +3214,40 @@
       <c r="Z8" s="2"/>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="3">
-        <v>339.0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1000.0</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="3">
-        <v>34144.0</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L9" s="1" t="s">
+      <c r="D9" s="6">
+        <v>413.0</v>
+      </c>
+      <c r="E9" s="6">
+        <v>3000.0</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="6">
+        <v>45394.0</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M9" s="2"/>
@@ -3271,41 +3266,41 @@
       <c r="Z9" s="2"/>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="3">
-        <v>69.0</v>
-      </c>
-      <c r="E10" s="3">
+      <c r="D10" s="6">
+        <v>84.0</v>
+      </c>
+      <c r="E10" s="6">
         <v>3680.0</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L10" s="3">
-        <v>2900.0</v>
+      <c r="F10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="6">
+        <v>3530.0</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -3323,41 +3318,41 @@
       <c r="Z10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="3">
-        <v>67.0</v>
-      </c>
-      <c r="E11" s="3">
+      <c r="D11" s="6">
+        <v>71.0</v>
+      </c>
+      <c r="E11" s="6">
         <v>2784.0</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" s="3">
-        <v>6.0</v>
-      </c>
-      <c r="L11" s="3">
-        <v>2346.0</v>
+      <c r="F11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="L11" s="6">
+        <v>2490.0</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -3375,40 +3370,40 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L12" s="1" t="s">
+      <c r="D12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M12" s="2"/>
@@ -3427,40 +3422,40 @@
       <c r="Z12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="3">
-        <v>86.0</v>
-      </c>
-      <c r="E13" s="3">
+      <c r="D13" s="6">
+        <v>90.0</v>
+      </c>
+      <c r="E13" s="6">
         <v>1635.0</v>
       </c>
-      <c r="F13" s="3">
-        <v>16200.0</v>
-      </c>
-      <c r="G13" s="3">
-        <v>581.0</v>
-      </c>
-      <c r="H13" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I13" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L13" s="1" t="s">
+      <c r="F13" s="6">
+        <v>18800.0</v>
+      </c>
+      <c r="G13" s="6">
+        <v>582.0</v>
+      </c>
+      <c r="H13" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="I13" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M13" s="2"/>
@@ -3479,40 +3474,40 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="3">
+      <c r="D14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="6">
         <v>65.0</v>
       </c>
-      <c r="H14" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="I14" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L14" s="1" t="s">
+      <c r="H14" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M14" s="2"/>
@@ -3531,40 +3526,40 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="3">
+      <c r="D15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="6">
         <v>169.0</v>
       </c>
-      <c r="H15" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="I15" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L15" s="1" t="s">
+      <c r="H15" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="I15" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L15" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M15" s="2"/>
@@ -3583,40 +3578,40 @@
       <c r="Z15" s="2"/>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="3">
+      <c r="D16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="6">
         <v>282.0</v>
       </c>
-      <c r="H16" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="I16" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L16" s="1" t="s">
+      <c r="H16" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="I16" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L16" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M16" s="2"/>
@@ -3635,40 +3630,40 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="3">
-        <v>1560.0</v>
-      </c>
-      <c r="H17" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="I17" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L17" s="1" t="s">
+      <c r="D17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1563.0</v>
+      </c>
+      <c r="H17" s="7">
+        <v>3.0</v>
+      </c>
+      <c r="I17" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L17" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M17" s="2"/>
@@ -3687,40 +3682,40 @@
       <c r="Z17" s="2"/>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="3">
-        <v>308.0</v>
-      </c>
-      <c r="E18" s="3">
-        <v>1000.0</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J18" s="3">
-        <v>27459.0</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L18" s="1" t="s">
+      <c r="D18" s="6">
+        <v>385.0</v>
+      </c>
+      <c r="E18" s="6">
+        <v>3000.0</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" s="6">
+        <v>34628.0</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L18" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M18" s="2"/>
@@ -3739,41 +3734,41 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="3">
-        <v>251.0</v>
-      </c>
-      <c r="E19" s="3">
+      <c r="D19" s="6">
+        <v>298.0</v>
+      </c>
+      <c r="E19" s="6">
         <v>3500.0</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L19" s="3">
-        <v>1540.0</v>
+      <c r="F19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L19" s="6">
+        <v>1910.0</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -3791,41 +3786,41 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="3">
-        <v>36.0</v>
-      </c>
-      <c r="E20" s="3">
+      <c r="D20" s="6">
+        <v>38.0</v>
+      </c>
+      <c r="E20" s="6">
         <v>8352.0</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K20" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="L20" s="3">
-        <v>2217.0</v>
+      <c r="F20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="L20" s="6">
+        <v>2280.0</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -3843,40 +3838,40 @@
       <c r="Z20" s="2"/>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="3">
-        <v>6.0</v>
-      </c>
-      <c r="H21" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I21" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L21" s="1" t="s">
+      <c r="D21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="H21" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="I21" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L21" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M21" s="2"/>
@@ -3895,40 +3890,40 @@
       <c r="Z21" s="2"/>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="6">
         <v>12.0</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="6">
         <v>2000.0</v>
       </c>
-      <c r="F22" s="3">
-        <v>24700.0</v>
-      </c>
-      <c r="G22" s="3">
+      <c r="F22" s="6">
+        <v>27600.0</v>
+      </c>
+      <c r="G22" s="6">
         <v>275.0</v>
       </c>
-      <c r="H22" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I22" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L22" s="1" t="s">
+      <c r="H22" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="I22" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L22" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M22" s="2"/>
@@ -3947,40 +3942,40 @@
       <c r="Z22" s="2"/>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" s="3">
-        <v>165.0</v>
-      </c>
-      <c r="H23" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="I23" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L23" s="1" t="s">
+      <c r="D23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="6">
+        <v>166.0</v>
+      </c>
+      <c r="H23" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="I23" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L23" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M23" s="2"/>
@@ -3999,40 +3994,40 @@
       <c r="Z23" s="2"/>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G24" s="3">
+      <c r="D24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="6">
         <v>398.0</v>
       </c>
-      <c r="H24" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="I24" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L24" s="1" t="s">
+      <c r="H24" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="I24" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L24" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M24" s="2"/>
@@ -4051,40 +4046,40 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G25" s="3">
-        <v>15.0</v>
-      </c>
-      <c r="H25" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="I25" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L25" s="1" t="s">
+      <c r="D25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="6">
+        <v>16.0</v>
+      </c>
+      <c r="H25" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="I25" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L25" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M25" s="2"/>
@@ -4130,6 +4125,20 @@
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
     </row>
+    <row r="27">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -4155,94 +4164,105 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>36</v>
       </c>
       <c r="J1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="C2" s="10">
+      <c r="B2" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="C2" s="11">
         <v>1.0</v>
       </c>
-      <c r="D2" s="11">
-        <v>4.0</v>
-      </c>
-      <c r="E2" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="G2" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="8" t="s">
+      <c r="D2" s="12">
+        <v>7.0</v>
+      </c>
+      <c r="E2" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="G2" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>15</v>
       </c>
       <c r="J2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="11">
-        <v>6.0</v>
-      </c>
-      <c r="D3" s="11">
-        <v>1432.0</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="11">
+      <c r="B3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="12">
+        <v>5.0</v>
+      </c>
+      <c r="D3" s="12">
+        <v>1437.0</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="12">
         <v>1.0</v>
       </c>
-      <c r="G3" s="11">
-        <v>565.0</v>
-      </c>
-      <c r="H3" s="11">
-        <v>0.0</v>
-      </c>
-      <c r="I3" s="11">
+      <c r="G3" s="12">
+        <v>566.0</v>
+      </c>
+      <c r="H3" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="I3" s="12">
         <v>0.0</v>
       </c>
       <c r="J3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>